<commit_message>
New Sheets Alert! participatingAgencies05232025pm.xlsx and pendingAgencies05232025pm.xlsx
</commit_message>
<xml_diff>
--- a/Pivot PendingAgencies/pivot-pendingAgencies05232025pm.xlsx
+++ b/Pivot PendingAgencies/pivot-pendingAgencies05232025pm.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,11 +450,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>New</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Present</t>
         </is>
       </c>
@@ -469,10 +464,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -487,9 +479,6 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -503,9 +492,6 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -519,9 +505,6 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -533,10 +516,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -549,9 +529,6 @@
         <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
         <v>4</v>
       </c>
     </row>
@@ -567,9 +544,6 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -581,9 +555,6 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -599,9 +570,6 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -613,9 +581,6 @@
         <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -631,9 +596,6 @@
       <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -645,9 +607,6 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -661,9 +620,6 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -677,9 +633,6 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -695,9 +648,6 @@
       <c r="C16" t="n">
         <v>0</v>
       </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -709,9 +659,6 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -727,9 +674,6 @@
       <c r="C18" t="n">
         <v>0</v>
       </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -743,9 +687,6 @@
       <c r="C19" t="n">
         <v>0</v>
       </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -757,9 +698,6 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
         <v>2</v>
       </c>
     </row>
@@ -775,9 +713,6 @@
       <c r="C21" t="n">
         <v>0</v>
       </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -791,9 +726,6 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -807,9 +739,6 @@
       <c r="C23" t="n">
         <v>0</v>
       </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -821,9 +750,6 @@
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -839,9 +765,6 @@
       <c r="C25" t="n">
         <v>0</v>
       </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -855,9 +778,6 @@
       <c r="C26" t="n">
         <v>0</v>
       </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -869,9 +789,6 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -885,9 +802,6 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -903,9 +817,6 @@
       <c r="C29" t="n">
         <v>0</v>
       </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -917,9 +828,6 @@
         <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
         <v>3</v>
       </c>
     </row>
@@ -933,9 +841,6 @@
         <v>27</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
         <v>4</v>
       </c>
     </row>
@@ -951,9 +856,6 @@
       <c r="C32" t="n">
         <v>0</v>
       </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -965,9 +867,6 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
         <v>7</v>
       </c>
     </row>
@@ -981,9 +880,6 @@
         <v>2</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
         <v>2</v>
       </c>
     </row>
@@ -997,9 +893,6 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1013,10 +906,7 @@
         <v>192</v>
       </c>
       <c r="C36" t="n">
-        <v>24</v>
-      </c>
-      <c r="D36" t="n">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>